<commit_message>
VT interconnect cable specs and w5500 test board
</commit_message>
<xml_diff>
--- a/hardware/VoltageTap_A/Meta VoltageTap A.xlsx
+++ b/hardware/VoltageTap_A/Meta VoltageTap A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\BeeMS\hardware\VoltageTap_A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09BA928-D31D-44FE-8A50-0EDE5A418C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4DED72-71D0-431A-AE51-087AE7C4C2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="0" windowWidth="29040" windowHeight="15840" xr2:uid="{E16E688C-64E3-4955-9FD3-F7092625115C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E16E688C-64E3-4955-9FD3-F7092625115C}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="2" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="157">
   <si>
     <t>last updated</t>
   </si>
@@ -516,6 +516,57 @@
   </si>
   <si>
     <t>expirementally determine ballancing circuit, include parts on next MB order</t>
+  </si>
+  <si>
+    <t>cool visual connector picker on mouser</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/c/i/?number%20of%20positions=8%20Position&amp;packaging=Tube&amp;pitch=2.54%20mm&amp;srsltid=AfmBOoo3AoR97TdMCuXKaB6ufQzjQTeWPaMW7V2CnTmUIDPGfkNKPkwc</t>
+  </si>
+  <si>
+    <t>EV.5.2.5 Each wire used in a Tractive Battery Container, whether it is part of the GLV or Tractive System, must be rated to the maximum Tractive System voltage</t>
+  </si>
+  <si>
+    <t>the intention is that wires don’t short</t>
+  </si>
+  <si>
+    <t>so we can have under specsed wires and connectors, as long as the cable length is 600v rated,, so heat shrink it</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Adam-Tech/FCS-08-SG?qs=xBpwZ0JX2zLXsIHjtia0ew%3D%3D&amp;srsltid=AfmBOoqg4eYgBt3YLFYUVTLoOpNtyC3yUxVKxfLNsrAAmEa31oEmFvKO</t>
+  </si>
+  <si>
+    <t>ribbon 8p 2x4 2.54mmp non latched, generic</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Wurth-Elektronik/61201022121?qs=ZtY9WdtwX54w6hXXLKx1qQ%3D%3D&amp;srsltid=AfmBOoohHCKYZ_5nThgnYgzjyJ7LWaEFKzoos-ZMx7nONpMAa6rFnMsR</t>
+  </si>
+  <si>
+    <t>10p 2.54mmp header latched wurth</t>
+  </si>
+  <si>
+    <t>50ft 8pin ribbon cable</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Pc-Accessories-Length-Conductors-Connectors/dp/B00E9P0F34</t>
+  </si>
+  <si>
+    <t>8p 2 wrap arround connector</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Wurth-Elektronik/61200823021?qs=PhR8RmCirEZvQm5v3EiYrA%3D%3D&amp;srsltid=AfmBOooMfGfO819iuGYG45dUWZESwH_55cLvg2yZ3m_V5O8BQQO5v-he</t>
+  </si>
+  <si>
+    <t>8p header right angle. Generic. Non latched</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Wurth-Elektronik/61200821721?qs=PhR8RmCirEb56BXUsQNR%2FQ%3D%3D&amp;srsltid=AfmBOooky3YWgEiw2M0jpH08etGmhJlXVmyZvnTkAkIslv9wCu9MU5VM</t>
+  </si>
+  <si>
+    <t>8p ribbon 1.25mmp 1m</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Wurth-Elektronik/63910815521CAB?qs=rrS6PyfT74fy4EdvcoRmTQ%3D%3D&amp;srsltid=AfmBOool47vkGpVeAHucxC0no_zWHdNkYm7E4z3ruE5nRaMYKgmp8BxC</t>
   </si>
 </sst>
 </file>
@@ -748,13 +799,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -775,16 +835,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1143,25 +1194,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BCE3943-DEC9-4765-B421-41457080BF0E}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43" style="2" customWidth="1"/>
     <col min="2" max="2" width="49.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>122</v>
       </c>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>123</v>
       </c>
@@ -1169,7 +1221,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>125</v>
       </c>
@@ -1178,7 +1230,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>126</v>
       </c>
@@ -1189,38 +1241,117 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="D5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="D6" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>139</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="11"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1269,11 +1400,11 @@
       <c r="M1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="L2" s="1" t="s">
@@ -1291,16 +1422,16 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
       <c r="J3" s="2" t="s">
         <v>60</v>
       </c>
@@ -1317,28 +1448,28 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="13"/>
+      <c r="H4" s="23"/>
       <c r="L4" s="1" t="s">
         <v>27</v>
       </c>
@@ -1348,12 +1479,12 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="15"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1556,16 +1687,16 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="23"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="16"/>
       <c r="L17" s="1" t="s">
         <v>40</v>
       </c>
@@ -1575,26 +1706,26 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="21" t="s">
+      <c r="F18" s="20"/>
+      <c r="G18" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H18" s="23"/>
+      <c r="H18" s="16"/>
       <c r="L18" s="1" t="s">
         <v>41</v>
       </c>
@@ -1604,12 +1735,12 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="19"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
       <c r="G19" s="4" t="s">
         <v>20</v>
       </c>
@@ -1734,8 +1865,8 @@
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="13"/>
       <c r="G25" s="1" t="s">
         <v>60</v>
       </c>
@@ -1755,8 +1886,8 @@
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="13"/>
       <c r="G26" s="1" t="s">
         <v>60</v>
       </c>
@@ -1776,8 +1907,8 @@
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="13"/>
       <c r="G27" s="1" t="s">
         <v>60</v>
       </c>
@@ -1797,8 +1928,8 @@
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="13"/>
       <c r="G28" s="1" t="s">
         <v>60</v>
       </c>
@@ -1818,8 +1949,8 @@
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="13"/>
       <c r="G29" s="1" t="s">
         <v>60</v>
       </c>
@@ -1839,8 +1970,8 @@
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="13"/>
       <c r="G30" s="1" t="s">
         <v>60</v>
       </c>
@@ -1865,16 +1996,16 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
       <c r="L32" s="1" t="s">
         <v>55</v>
       </c>
@@ -1884,26 +2015,26 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="13" t="s">
+      <c r="F33" s="20"/>
+      <c r="G33" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="H33" s="13"/>
+      <c r="H33" s="23"/>
       <c r="L33" s="1" t="s">
         <v>56</v>
       </c>
@@ -1913,12 +2044,12 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="19"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="22"/>
       <c r="G34" s="4" t="s">
         <v>20</v>
       </c>
@@ -1946,10 +2077,10 @@
       <c r="D35" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="F35" s="12"/>
+      <c r="F35" s="13"/>
       <c r="G35" s="1" t="s">
         <v>60</v>
       </c>
@@ -1977,10 +2108,10 @@
       <c r="D36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="F36" s="12"/>
+      <c r="F36" s="13"/>
       <c r="G36" s="1" t="s">
         <v>60</v>
       </c>
@@ -2008,10 +2139,10 @@
       <c r="D37" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="F37" s="12"/>
+      <c r="F37" s="13"/>
       <c r="G37" s="1" t="s">
         <v>60</v>
       </c>
@@ -2039,10 +2170,10 @@
       <c r="D38" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="F38" s="12"/>
+      <c r="F38" s="13"/>
       <c r="G38" s="1" t="s">
         <v>60</v>
       </c>
@@ -2070,8 +2201,8 @@
       <c r="D39" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="11"/>
-      <c r="F39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="13"/>
       <c r="G39" s="1" t="s">
         <v>60</v>
       </c>
@@ -2099,8 +2230,8 @@
       <c r="D40" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="13"/>
       <c r="G40" s="1" t="s">
         <v>60</v>
       </c>
@@ -2128,8 +2259,8 @@
       <c r="D41" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="11"/>
-      <c r="F41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="13"/>
       <c r="G41" s="1" t="s">
         <v>60</v>
       </c>
@@ -2157,8 +2288,8 @@
       <c r="D42" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="11"/>
-      <c r="F42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="13"/>
       <c r="G42" s="1" t="s">
         <v>60</v>
       </c>
@@ -2186,8 +2317,8 @@
       <c r="D43" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E43" s="11"/>
-      <c r="F43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="13"/>
       <c r="G43" s="1" t="s">
         <v>60</v>
       </c>
@@ -2215,8 +2346,8 @@
       <c r="D44" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="13"/>
       <c r="G44" s="1" t="s">
         <v>60</v>
       </c>
@@ -2244,8 +2375,8 @@
       <c r="D45" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="11"/>
-      <c r="F45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="13"/>
       <c r="G45" s="1" t="s">
         <v>60</v>
       </c>
@@ -2273,10 +2404,10 @@
       <c r="D46" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="E46" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F46" s="12"/>
+      <c r="F46" s="13"/>
       <c r="G46" s="1" t="s">
         <v>60</v>
       </c>
@@ -2304,10 +2435,10 @@
       <c r="D47" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="E47" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F47" s="12"/>
+      <c r="F47" s="13"/>
       <c r="G47" s="1" t="s">
         <v>60</v>
       </c>
@@ -2335,10 +2466,10 @@
       <c r="D48" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="E48" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F48" s="12"/>
+      <c r="F48" s="13"/>
       <c r="G48" s="1" t="s">
         <v>60</v>
       </c>
@@ -2364,8 +2495,8 @@
       <c r="D49" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E49" s="11"/>
-      <c r="F49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="13"/>
       <c r="G49" s="1" t="s">
         <v>60</v>
       </c>
@@ -2391,10 +2522,10 @@
       <c r="D50" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="E50" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="F50" s="12"/>
+      <c r="F50" s="13"/>
       <c r="G50" s="1" t="s">
         <v>60</v>
       </c>
@@ -2420,10 +2551,10 @@
       <c r="D51" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="E51" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="F51" s="12"/>
+      <c r="F51" s="13"/>
       <c r="G51" s="1" t="s">
         <v>60</v>
       </c>
@@ -2449,8 +2580,8 @@
       <c r="D52" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E52" s="11"/>
-      <c r="F52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="13"/>
       <c r="G52" s="1" t="s">
         <v>60</v>
       </c>
@@ -2476,8 +2607,8 @@
       <c r="D53" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E53" s="11"/>
-      <c r="F53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="13"/>
       <c r="G53" s="1" t="s">
         <v>60</v>
       </c>
@@ -2503,8 +2634,8 @@
       <c r="D54" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E54" s="11"/>
-      <c r="F54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="13"/>
       <c r="G54" s="1" t="s">
         <v>60</v>
       </c>
@@ -2522,8 +2653,8 @@
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="13"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="L55" s="1"/>
@@ -2537,8 +2668,8 @@
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="13"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="L56" s="1"/>
@@ -2552,8 +2683,8 @@
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="13"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="L57" s="1"/>
@@ -2567,8 +2698,8 @@
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="13"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="L58" s="1"/>
@@ -2636,6 +2767,43 @@
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="A32:H32"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:F34"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:F19"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="E56:F56"/>
     <mergeCell ref="E57:F57"/>
@@ -2652,43 +2820,6 @@
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="G18:H18"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:F34"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="A32:H32"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="A33:A34"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="K3">

</xml_diff>